<commit_message>
modified:   excel_operate/__pycache__/__init__.cpython-310.pyc 	modified:   "tests/\347\244\272\344\276\213 - \344\277\256\346\224\271.xlsx"
</commit_message>
<xml_diff>
--- a/tests/示例 - 修改.xlsx
+++ b/tests/示例 - 修改.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="工作表 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="工作表 2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="工作表 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="工作表 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="工作表 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="工作表 3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>

</xml_diff>